<commit_message>
Update demographic model results
</commit_message>
<xml_diff>
--- a/Figures_data/fastsimcoal2/Total_Cassiope_bestlhoods_bottlenecks.xlsx
+++ b/Figures_data/fastsimcoal2/Total_Cassiope_bestlhoods_bottlenecks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\Documents\GitHub\Population_genomics_Cassiope\Figures_data\fastsimcoal2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4F801EF-0835-4296-8236-0CED75397BD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0507125-A329-45D7-9EAE-42B821E98A3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="887" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="38">
   <si>
     <t>N_Europe</t>
   </si>
@@ -124,6 +124,33 @@
   </si>
   <si>
     <t>Tetragona Greenland  Bottleneck - Model D</t>
+  </si>
+  <si>
+    <t>TDIVEurAla_kyrs</t>
+  </si>
+  <si>
+    <t>TDIVRusAla_kyrs</t>
+  </si>
+  <si>
+    <t>TDIVSaxTet_kyrs</t>
+  </si>
+  <si>
+    <t>TDIVGreEur_kyrs</t>
+  </si>
+  <si>
+    <t>TDIVEurAla_gen</t>
+  </si>
+  <si>
+    <t>TDIVRusAla_gen</t>
+  </si>
+  <si>
+    <t>TDIVSaxTet_gen</t>
+  </si>
+  <si>
+    <t>TDIVGreEur_gen</t>
+  </si>
+  <si>
+    <t>TDIVGre Eur_gen</t>
   </si>
 </sst>
 </file>
@@ -613,12 +640,35 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="11" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -997,14 +1047,24 @@
   <dimension ref="A1:S20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20:R20"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="17" max="17" width="11.109375" customWidth="1"/>
-    <col min="18" max="18" width="11.6640625" customWidth="1"/>
-    <col min="19" max="19" width="11" customWidth="1"/>
+    <col min="1" max="3" width="8.88671875" style="5"/>
+    <col min="4" max="4" width="13.77734375" style="5" customWidth="1"/>
+    <col min="5" max="5" width="13.88671875" style="5" customWidth="1"/>
+    <col min="6" max="6" width="9.88671875" style="5" customWidth="1"/>
+    <col min="7" max="7" width="8" style="5" customWidth="1"/>
+    <col min="8" max="8" width="7.88671875" style="5" customWidth="1"/>
+    <col min="9" max="9" width="8.21875" style="5" customWidth="1"/>
+    <col min="10" max="13" width="8.88671875" style="5"/>
+    <col min="14" max="14" width="8.21875" style="5" customWidth="1"/>
+    <col min="15" max="15" width="8.88671875" style="5"/>
+    <col min="16" max="16" width="7.5546875" style="5" customWidth="1"/>
+    <col min="17" max="17" width="7.88671875" style="5" customWidth="1"/>
+    <col min="18" max="19" width="7.77734375" style="5" customWidth="1"/>
     <col min="21" max="21" width="11.6640625" customWidth="1"/>
     <col min="22" max="22" width="12.6640625" customWidth="1"/>
     <col min="23" max="23" width="11.77734375" customWidth="1"/>
@@ -1012,977 +1072,1026 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="4" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:19" s="3" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="J2" s="3" t="s">
+      <c r="G2" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="H2" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="I2" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="J2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="K2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="L2" s="3" t="s">
+      <c r="L2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="M2" s="3" t="s">
+      <c r="M2" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="N2" s="3" t="s">
+      <c r="N2" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="O2" s="3" t="s">
+      <c r="O2" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="Q2" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="R2" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="S2" s="3" t="s">
-        <v>8</v>
+      <c r="P2" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q2" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="R2" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="S2" s="10" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A3">
+      <c r="A3" s="5">
         <v>657998</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="5">
         <v>942386</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="5">
         <v>614455</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="5">
         <v>814235</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="11">
         <v>192364</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="11">
         <v>4061317</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="11">
         <v>22330</v>
       </c>
-      <c r="H3">
+      <c r="H3" s="11">
         <v>81799</v>
       </c>
-      <c r="I3">
+      <c r="I3" s="11">
         <v>596610</v>
       </c>
-      <c r="J3">
+      <c r="J3" s="7">
         <v>0.19166320000000001</v>
       </c>
-      <c r="K3">
+      <c r="K3" s="7">
         <v>0.1230979</v>
       </c>
-      <c r="L3">
+      <c r="L3" s="7">
         <v>0.26298240000000001</v>
       </c>
-      <c r="M3">
+      <c r="M3" s="7">
         <v>3.5597400000000001E-2</v>
       </c>
-      <c r="N3">
+      <c r="N3" s="5">
         <v>-9831.4110000000001</v>
       </c>
-      <c r="O3">
+      <c r="O3" s="5">
         <v>-8446.5319999999992</v>
       </c>
-      <c r="P3">
+      <c r="P3" s="5">
         <f>O3-N3</f>
         <v>1384.8790000000008</v>
       </c>
-      <c r="Q3">
+      <c r="Q3" s="11">
         <f t="shared" ref="Q3:S5" si="0">G3*10/1000</f>
         <v>223.3</v>
       </c>
-      <c r="R3">
+      <c r="R3" s="11">
         <f t="shared" si="0"/>
         <v>817.99</v>
       </c>
-      <c r="S3">
+      <c r="S3" s="11">
         <f t="shared" si="0"/>
         <v>5966.1</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A4">
+      <c r="A4" s="5">
         <v>224119</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="5">
         <v>990996</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="5">
         <v>379775</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="5">
         <v>910799</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="11">
         <v>222405</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="11">
         <v>4017216</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="11">
         <v>12745</v>
       </c>
-      <c r="H4">
+      <c r="H4" s="11">
         <v>104599</v>
       </c>
-      <c r="I4">
+      <c r="I4" s="11">
         <v>633123</v>
       </c>
-      <c r="J4">
+      <c r="J4" s="7">
         <v>0.10814550000000001</v>
       </c>
-      <c r="K4">
+      <c r="K4" s="7">
         <v>0.10748530000000001</v>
       </c>
-      <c r="L4">
+      <c r="L4" s="7">
         <v>0.62014840000000004</v>
       </c>
-      <c r="M4">
+      <c r="M4" s="7">
         <v>0.1045896</v>
       </c>
-      <c r="N4">
+      <c r="N4" s="5">
         <v>-9826.5120000000006</v>
       </c>
-      <c r="O4">
+      <c r="O4" s="5">
         <v>-8446.5319999999992</v>
       </c>
-      <c r="P4">
+      <c r="P4" s="5">
         <f>O4-N4</f>
         <v>1379.9800000000014</v>
       </c>
-      <c r="Q4">
+      <c r="Q4" s="11">
         <f t="shared" si="0"/>
         <v>127.45</v>
       </c>
-      <c r="R4">
+      <c r="R4" s="11">
         <f t="shared" si="0"/>
         <v>1045.99</v>
       </c>
-      <c r="S4">
+      <c r="S4" s="11">
         <f t="shared" si="0"/>
         <v>6331.23</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A5" s="2">
+      <c r="A5" s="6">
         <v>324389</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5" s="6">
         <v>906851</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" s="6">
         <v>351212</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5" s="6">
         <v>900070</v>
       </c>
-      <c r="E5" s="2">
+      <c r="E5" s="12">
         <v>151964</v>
       </c>
-      <c r="F5" s="2">
+      <c r="F5" s="12">
         <v>4677409</v>
       </c>
-      <c r="G5" s="2">
+      <c r="G5" s="12">
         <v>37923</v>
       </c>
-      <c r="H5" s="2">
+      <c r="H5" s="12">
         <v>68170</v>
       </c>
-      <c r="I5" s="2">
+      <c r="I5" s="12">
         <v>540182</v>
       </c>
-      <c r="J5" s="2">
+      <c r="J5" s="8">
         <v>0.103002</v>
       </c>
-      <c r="K5" s="2">
+      <c r="K5" s="8">
         <v>3.6628800000000003E-2</v>
       </c>
-      <c r="L5" s="2">
+      <c r="L5" s="8">
         <v>8.3227999999999996E-2</v>
       </c>
-      <c r="M5" s="2">
+      <c r="M5" s="8">
         <v>0.22371360000000001</v>
       </c>
-      <c r="N5" s="2">
+      <c r="N5" s="6">
         <v>-9794.1640000000007</v>
       </c>
-      <c r="O5" s="2">
+      <c r="O5" s="6">
         <v>-8446.5319999999992</v>
       </c>
-      <c r="P5" s="2">
+      <c r="P5" s="6">
         <f>O5-N5</f>
         <v>1347.6320000000014</v>
       </c>
-      <c r="Q5" s="2">
+      <c r="Q5" s="12">
         <f t="shared" si="0"/>
         <v>379.23</v>
       </c>
-      <c r="R5" s="2">
+      <c r="R5" s="12">
         <f t="shared" si="0"/>
         <v>681.7</v>
       </c>
-      <c r="S5" s="2">
+      <c r="S5" s="12">
         <f t="shared" si="0"/>
         <v>5401.82</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="4" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="7" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="3" t="s">
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="11"/>
+      <c r="I6" s="11"/>
+      <c r="Q6" s="11"/>
+      <c r="R6" s="11"/>
+      <c r="S6" s="11"/>
+    </row>
+    <row r="7" spans="1:19" s="3" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A7" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="E7" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="F7" s="3" t="s">
+      <c r="F7" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="G7" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="H7" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="I7" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="J7" s="3" t="s">
+      <c r="G7" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="H7" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="I7" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="J7" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="K7" s="3" t="s">
+      <c r="K7" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="L7" s="3" t="s">
+      <c r="L7" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="M7" s="3" t="s">
+      <c r="M7" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="N7" s="3" t="s">
+      <c r="N7" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="O7" s="3" t="s">
+      <c r="O7" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="P7" s="3" t="s">
+      <c r="P7" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="Q7" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="R7" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="S7" s="3" t="s">
-        <v>7</v>
+      <c r="Q7" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="R7" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="S7" s="10" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A8">
+      <c r="A8" s="5">
         <v>176675</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="5">
         <v>833474</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="5">
         <v>370965</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="5">
         <v>907121</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="11">
         <v>917166</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="11">
         <v>4678221</v>
       </c>
-      <c r="G8">
+      <c r="G8" s="11">
         <v>4798</v>
       </c>
-      <c r="H8">
+      <c r="H8" s="11">
         <v>26702</v>
       </c>
-      <c r="I8">
+      <c r="I8" s="11">
         <v>124756</v>
       </c>
-      <c r="J8">
+      <c r="J8" s="7">
         <v>0.2352901</v>
       </c>
-      <c r="K8">
+      <c r="K8" s="7">
         <v>0.75936700000000001</v>
       </c>
-      <c r="L8">
+      <c r="L8" s="7">
         <v>0.30861250000000001</v>
       </c>
-      <c r="M8">
+      <c r="M8" s="7">
         <v>0.34043980000000001</v>
       </c>
-      <c r="N8">
+      <c r="N8" s="5">
         <v>-8444.7810000000009</v>
       </c>
-      <c r="O8">
+      <c r="O8" s="5">
         <v>-7410.1310000000003</v>
       </c>
-      <c r="P8">
+      <c r="P8" s="5">
         <f>O8-N8</f>
         <v>1034.6500000000005</v>
       </c>
-      <c r="Q8">
+      <c r="Q8" s="11">
         <f t="shared" ref="Q8:S10" si="1">G8*10/1000</f>
         <v>47.98</v>
       </c>
-      <c r="R8">
+      <c r="R8" s="11">
         <f t="shared" si="1"/>
         <v>267.02</v>
       </c>
-      <c r="S8">
+      <c r="S8" s="11">
         <f t="shared" si="1"/>
         <v>1247.56</v>
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A9">
+      <c r="A9" s="5">
         <v>298657</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="5">
         <v>901481</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="5">
         <v>378470</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="5">
         <v>831240</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="11">
         <v>154470</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="11">
         <v>4965145</v>
       </c>
-      <c r="G9">
+      <c r="G9" s="11">
         <v>8026</v>
       </c>
-      <c r="H9">
+      <c r="H9" s="11">
         <v>26537</v>
       </c>
-      <c r="I9">
+      <c r="I9" s="11">
         <v>103604</v>
       </c>
-      <c r="J9">
+      <c r="J9" s="7">
         <v>0.27324500000000002</v>
       </c>
-      <c r="K9">
+      <c r="K9" s="7">
         <v>0.68407629999999997</v>
       </c>
-      <c r="L9">
+      <c r="L9" s="7">
         <v>0.26156750000000001</v>
       </c>
-      <c r="M9">
+      <c r="M9" s="7">
         <v>0.5183373</v>
       </c>
-      <c r="N9">
+      <c r="N9" s="5">
         <v>-8439.7950000000001</v>
       </c>
-      <c r="O9">
+      <c r="O9" s="5">
         <v>-7410.1310000000003</v>
       </c>
-      <c r="P9">
+      <c r="P9" s="5">
         <f t="shared" ref="P9:P20" si="2">O9-N9</f>
         <v>1029.6639999999998</v>
       </c>
-      <c r="Q9">
+      <c r="Q9" s="11">
         <f t="shared" si="1"/>
         <v>80.260000000000005</v>
       </c>
-      <c r="R9">
+      <c r="R9" s="11">
         <f t="shared" si="1"/>
         <v>265.37</v>
       </c>
-      <c r="S9">
+      <c r="S9" s="11">
         <f t="shared" si="1"/>
         <v>1036.04</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A10" s="2">
+      <c r="A10" s="6">
         <v>214339</v>
       </c>
-      <c r="B10" s="2">
+      <c r="B10" s="6">
         <v>943677</v>
       </c>
-      <c r="C10" s="2">
+      <c r="C10" s="6">
         <v>351511</v>
       </c>
-      <c r="D10" s="2">
+      <c r="D10" s="6">
         <v>866907</v>
       </c>
-      <c r="E10" s="2">
+      <c r="E10" s="12">
         <v>149809</v>
       </c>
-      <c r="F10" s="2">
+      <c r="F10" s="12">
         <v>5045312</v>
       </c>
-      <c r="G10" s="2">
+      <c r="G10" s="12">
         <v>4464</v>
       </c>
-      <c r="H10" s="2">
+      <c r="H10" s="12">
         <v>19924</v>
       </c>
-      <c r="I10" s="2">
+      <c r="I10" s="12">
         <v>125961</v>
       </c>
-      <c r="J10" s="2">
+      <c r="J10" s="8">
         <v>0.52053320000000003</v>
       </c>
-      <c r="K10" s="2">
+      <c r="K10" s="8">
         <v>0.60738139999999996</v>
       </c>
-      <c r="L10" s="2">
+      <c r="L10" s="8">
         <v>0.74382789999999999</v>
       </c>
-      <c r="M10" s="2">
+      <c r="M10" s="8">
         <v>0.61039489999999996</v>
       </c>
-      <c r="N10" s="2">
+      <c r="N10" s="6">
         <v>-8426.4220000000005</v>
       </c>
-      <c r="O10" s="2">
+      <c r="O10" s="6">
         <v>-7410.1310000000003</v>
       </c>
-      <c r="P10" s="2">
+      <c r="P10" s="6">
         <f t="shared" si="2"/>
         <v>1016.2910000000002</v>
       </c>
-      <c r="Q10" s="2">
+      <c r="Q10" s="12">
         <f t="shared" si="1"/>
         <v>44.64</v>
       </c>
-      <c r="R10" s="2">
+      <c r="R10" s="12">
         <f t="shared" si="1"/>
         <v>199.24</v>
       </c>
-      <c r="S10" s="2">
+      <c r="S10" s="12">
         <f t="shared" si="1"/>
         <v>1259.6099999999999</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A11" s="3" t="s">
+      <c r="A11" s="4" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="12" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="3" t="s">
+      <c r="E11" s="11"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="11"/>
+      <c r="H11" s="11"/>
+      <c r="I11" s="11"/>
+      <c r="J11" s="7"/>
+      <c r="K11" s="7"/>
+      <c r="L11" s="7"/>
+      <c r="M11" s="7"/>
+      <c r="Q11" s="11"/>
+      <c r="R11" s="11"/>
+      <c r="S11" s="11"/>
+    </row>
+    <row r="12" spans="1:19" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A12" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="D12" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="E12" s="3" t="s">
+      <c r="E12" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="F12" s="3" t="s">
+      <c r="F12" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="G12" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="H12" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="I12" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="J12" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="K12" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="L12" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="M12" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="N12" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="O12" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="P12" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q12" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="G12" s="3" t="s">
+      <c r="R12" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="H12" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="I12" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="J12" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="K12" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="L12" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="M12" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="N12" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="O12" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q12" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="R12" s="3" t="s">
-        <v>7</v>
-      </c>
+      <c r="S12" s="10"/>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A13">
+      <c r="A13" s="5">
         <v>409597</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="5">
         <v>2818871</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="5">
         <v>771355</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="5">
         <v>11189</v>
       </c>
-      <c r="E13">
+      <c r="E13" s="11">
         <v>164374</v>
       </c>
-      <c r="F13">
+      <c r="F13" s="11">
         <v>63256</v>
       </c>
-      <c r="G13">
+      <c r="G13" s="11">
         <v>220622</v>
       </c>
-      <c r="H13">
+      <c r="H13" s="13">
         <v>1.56136E-2</v>
       </c>
-      <c r="I13">
+      <c r="I13" s="13">
         <v>1.7148099999999999E-2</v>
       </c>
-      <c r="J13">
+      <c r="J13" s="7">
         <v>7.8898800000000005E-2</v>
       </c>
-      <c r="K13">
+      <c r="K13" s="7">
         <v>7.0893300000000006E-2</v>
       </c>
-      <c r="L13">
+      <c r="L13" s="7">
         <v>1.0552444000000001</v>
       </c>
-      <c r="M13">
+      <c r="M13" s="7">
         <v>0.48431390000000002</v>
       </c>
-      <c r="N13">
+      <c r="N13" s="5">
         <v>-7115.6360000000004</v>
       </c>
-      <c r="O13">
+      <c r="O13" s="5">
         <v>-6864.5540000000001</v>
       </c>
-      <c r="P13">
+      <c r="P13" s="5">
         <f t="shared" si="2"/>
         <v>251.08200000000033</v>
       </c>
-      <c r="Q13">
+      <c r="Q13" s="11">
         <f t="shared" ref="Q13:R15" si="3">F13*10/1000</f>
         <v>632.55999999999995</v>
       </c>
-      <c r="R13">
+      <c r="R13" s="11">
         <f t="shared" si="3"/>
         <v>2206.2199999999998</v>
       </c>
+      <c r="S13" s="11"/>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A14">
+      <c r="A14" s="5">
         <v>329647</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="5">
         <v>2325545</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="5">
         <v>627323</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="5">
         <v>750270</v>
       </c>
-      <c r="E14">
+      <c r="E14" s="11">
         <v>6869</v>
       </c>
-      <c r="F14">
+      <c r="F14" s="11">
         <v>51893</v>
       </c>
-      <c r="G14">
+      <c r="G14" s="11">
         <v>177309</v>
       </c>
-      <c r="H14">
+      <c r="H14" s="13">
         <v>2.1682699999999999E-2</v>
       </c>
-      <c r="I14">
+      <c r="I14" s="13">
         <v>2.82064E-2</v>
       </c>
-      <c r="J14">
+      <c r="J14" s="7">
         <v>0.1331147</v>
       </c>
-      <c r="K14">
+      <c r="K14" s="7">
         <v>4.2056000000000003E-2</v>
       </c>
-      <c r="L14">
+      <c r="L14" s="7">
         <v>0.57873669999999999</v>
       </c>
-      <c r="M14">
+      <c r="M14" s="7">
         <v>0.39340530000000001</v>
       </c>
-      <c r="N14">
+      <c r="N14" s="5">
         <v>-7115.2709999999997</v>
       </c>
-      <c r="O14">
+      <c r="O14" s="5">
         <v>-6864.5540000000001</v>
       </c>
-      <c r="P14">
+      <c r="P14" s="5">
         <f t="shared" si="2"/>
         <v>250.71699999999964</v>
       </c>
-      <c r="Q14">
+      <c r="Q14" s="11">
         <f t="shared" si="3"/>
         <v>518.92999999999995</v>
       </c>
-      <c r="R14">
+      <c r="R14" s="11">
         <f t="shared" si="3"/>
         <v>1773.09</v>
       </c>
+      <c r="S14" s="11"/>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A15" s="2">
+      <c r="A15" s="6">
         <v>149623</v>
       </c>
-      <c r="B15" s="2">
+      <c r="B15" s="6">
         <v>1238723</v>
       </c>
-      <c r="C15" s="2">
+      <c r="C15" s="6">
         <v>324674</v>
       </c>
-      <c r="D15" s="2">
+      <c r="D15" s="6">
         <v>228212</v>
       </c>
-      <c r="E15" s="2">
+      <c r="E15" s="12">
         <v>2337</v>
       </c>
-      <c r="F15" s="2">
+      <c r="F15" s="12">
         <v>21350</v>
       </c>
-      <c r="G15" s="2">
+      <c r="G15" s="12">
         <v>95525</v>
       </c>
-      <c r="H15" s="2">
+      <c r="H15" s="14">
         <v>2.8448000000000002E-3</v>
       </c>
-      <c r="I15" s="2">
+      <c r="I15" s="14">
         <v>5.7718999999999999E-3</v>
       </c>
-      <c r="J15" s="2">
+      <c r="J15" s="8">
         <v>2.3664000000000001E-2</v>
       </c>
-      <c r="K15" s="2">
+      <c r="K15" s="8">
         <v>7.7519000000000005E-2</v>
       </c>
-      <c r="L15" s="2">
+      <c r="L15" s="8">
         <v>0.65125429999999995</v>
       </c>
-      <c r="M15" s="2">
+      <c r="M15" s="8">
         <v>0.3710369</v>
       </c>
-      <c r="N15" s="2">
+      <c r="N15" s="6">
         <v>-7104.2780000000002</v>
       </c>
-      <c r="O15" s="2">
+      <c r="O15" s="6">
         <v>-6864.5540000000001</v>
       </c>
-      <c r="P15" s="2">
+      <c r="P15" s="6">
         <f t="shared" si="2"/>
         <v>239.72400000000016</v>
       </c>
-      <c r="Q15" s="2">
+      <c r="Q15" s="12">
         <f t="shared" si="3"/>
         <v>213.5</v>
       </c>
-      <c r="R15" s="2">
+      <c r="R15" s="12">
         <f t="shared" si="3"/>
         <v>955.25</v>
       </c>
+      <c r="S15" s="11"/>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A16" s="3" t="s">
+      <c r="A16" s="4" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="17" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="3" t="s">
+      <c r="E16" s="11"/>
+      <c r="F16" s="11"/>
+      <c r="G16" s="11"/>
+      <c r="H16" s="13"/>
+      <c r="I16" s="13"/>
+      <c r="J16" s="7"/>
+      <c r="K16" s="7"/>
+      <c r="L16" s="7"/>
+      <c r="M16" s="7"/>
+      <c r="Q16" s="11"/>
+      <c r="R16" s="11"/>
+      <c r="S16" s="11"/>
+    </row>
+    <row r="17" spans="1:19" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A17" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B17" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="C17" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D17" s="3" t="s">
+      <c r="D17" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="E17" s="3" t="s">
+      <c r="E17" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="F17" s="3" t="s">
+      <c r="F17" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="G17" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="H17" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="I17" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="J17" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="K17" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="L17" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="M17" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="N17" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="O17" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="P17" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q17" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="G17" s="3" t="s">
+      <c r="R17" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="H17" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="I17" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="J17" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="K17" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="L17" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="M17" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="N17" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="O17" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q17" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="R17" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A18">
+      <c r="S17" s="10"/>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A18" s="5">
         <v>691411</v>
       </c>
-      <c r="B18">
+      <c r="B18" s="5">
         <v>2768466</v>
       </c>
-      <c r="C18">
+      <c r="C18" s="5">
         <v>33642</v>
       </c>
-      <c r="D18">
+      <c r="D18" s="5">
         <v>301740</v>
       </c>
-      <c r="E18">
+      <c r="E18" s="11">
         <v>1723</v>
       </c>
-      <c r="F18">
+      <c r="F18" s="11">
         <v>92716</v>
       </c>
-      <c r="G18">
+      <c r="G18" s="11">
         <v>6068</v>
       </c>
-      <c r="H18">
+      <c r="H18" s="13">
         <v>2.6416E-3</v>
       </c>
-      <c r="I18">
+      <c r="I18" s="13">
         <v>7.2312000000000001E-3</v>
       </c>
-      <c r="J18">
+      <c r="J18" s="7">
         <v>1.69132E-2</v>
       </c>
-      <c r="K18">
+      <c r="K18" s="7">
         <v>3.6564199999999998E-2</v>
       </c>
-      <c r="L18">
+      <c r="L18" s="7">
         <v>0.72759759999999996</v>
       </c>
-      <c r="M18">
+      <c r="M18" s="7">
         <v>0.32294509999999998</v>
       </c>
-      <c r="N18">
+      <c r="N18" s="5">
         <v>-5653.2939999999999</v>
       </c>
-      <c r="O18">
+      <c r="O18" s="5">
         <v>-5522.2190000000001</v>
       </c>
-      <c r="P18">
+      <c r="P18" s="5">
         <f t="shared" si="2"/>
         <v>131.07499999999982</v>
       </c>
-      <c r="Q18">
+      <c r="Q18" s="11">
         <f t="shared" ref="Q18:R20" si="4">F18*10/1000</f>
         <v>927.16</v>
       </c>
-      <c r="R18">
+      <c r="R18" s="11">
         <f t="shared" si="4"/>
         <v>60.68</v>
       </c>
-    </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A19">
+      <c r="S18" s="11"/>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A19" s="5">
         <v>654670</v>
       </c>
-      <c r="B19">
+      <c r="B19" s="5">
         <v>2401312</v>
       </c>
-      <c r="C19">
+      <c r="C19" s="5">
         <v>37453</v>
       </c>
-      <c r="D19">
+      <c r="D19" s="5">
         <v>16010</v>
       </c>
-      <c r="E19">
+      <c r="E19" s="11">
         <v>12731</v>
       </c>
-      <c r="F19">
+      <c r="F19" s="11">
         <v>82661</v>
       </c>
-      <c r="G19">
+      <c r="G19" s="11">
         <v>6546</v>
       </c>
-      <c r="H19" s="1">
+      <c r="H19" s="13">
         <v>4.26523E-4</v>
       </c>
-      <c r="I19" s="1">
+      <c r="I19" s="13">
         <v>8.2996399999999998E-4</v>
       </c>
-      <c r="J19">
+      <c r="J19" s="7">
         <v>1.42084E-2</v>
       </c>
-      <c r="K19">
+      <c r="K19" s="7">
         <v>2.7869100000000001E-2</v>
       </c>
-      <c r="L19">
+      <c r="L19" s="7">
         <v>0.69458770000000003</v>
       </c>
-      <c r="M19">
+      <c r="M19" s="7">
         <v>0.83192469999999996</v>
       </c>
-      <c r="N19">
+      <c r="N19" s="5">
         <v>-5591.2790000000005</v>
       </c>
-      <c r="O19">
+      <c r="O19" s="5">
         <v>-5522.2190000000001</v>
       </c>
-      <c r="P19">
+      <c r="P19" s="5">
         <f t="shared" si="2"/>
         <v>69.0600000000004</v>
       </c>
-      <c r="Q19">
+      <c r="Q19" s="11">
         <f t="shared" si="4"/>
         <v>826.61</v>
       </c>
-      <c r="R19">
+      <c r="R19" s="11">
         <f t="shared" si="4"/>
         <v>65.459999999999994</v>
       </c>
-    </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A20" s="2">
+      <c r="S19" s="11"/>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A20" s="6">
         <v>635041</v>
       </c>
-      <c r="B20" s="2">
+      <c r="B20" s="6">
         <v>2226340</v>
       </c>
-      <c r="C20" s="2">
+      <c r="C20" s="6">
         <v>31907</v>
       </c>
-      <c r="D20" s="2">
+      <c r="D20" s="6">
         <v>14731</v>
       </c>
-      <c r="E20" s="2">
+      <c r="E20" s="12">
         <v>13602</v>
       </c>
-      <c r="F20" s="2">
+      <c r="F20" s="12">
         <v>77951</v>
       </c>
-      <c r="G20" s="2">
+      <c r="G20" s="12">
         <v>5498</v>
       </c>
-      <c r="H20" s="4">
+      <c r="H20" s="14">
         <v>3.2394699999999999E-4</v>
       </c>
-      <c r="I20" s="4">
+      <c r="I20" s="14">
         <v>7.99171E-4</v>
       </c>
-      <c r="J20" s="2">
+      <c r="J20" s="8">
         <v>1.6523199999999998E-2</v>
       </c>
-      <c r="K20" s="2">
+      <c r="K20" s="8">
         <v>1.9569199999999998E-2</v>
       </c>
-      <c r="L20" s="2">
+      <c r="L20" s="8">
         <v>0.37816549999999999</v>
       </c>
-      <c r="M20" s="2">
+      <c r="M20" s="8">
         <v>0.64795400000000003</v>
       </c>
-      <c r="N20" s="2">
+      <c r="N20" s="6">
         <v>-5590.701</v>
       </c>
-      <c r="O20" s="2">
+      <c r="O20" s="6">
         <v>-5522.2190000000001</v>
       </c>
-      <c r="P20" s="2">
+      <c r="P20" s="6">
         <f t="shared" si="2"/>
         <v>68.481999999999971</v>
       </c>
-      <c r="Q20" s="2">
+      <c r="Q20" s="12">
         <f t="shared" si="4"/>
         <v>779.51</v>
       </c>
-      <c r="R20" s="2">
+      <c r="R20" s="12">
         <f t="shared" si="4"/>
         <v>54.98</v>
       </c>
+      <c r="S20" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Add sample size plots pi and FST
</commit_message>
<xml_diff>
--- a/Figures_data/fastsimcoal2/Total_Cassiope_bestlhoods_bottlenecks.xlsx
+++ b/Figures_data/fastsimcoal2/Total_Cassiope_bestlhoods_bottlenecks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\Documents\GitHub\Population_genomics_Cassiope\Figures_data\fastsimcoal2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0507125-A329-45D7-9EAE-42B821E98A3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{305309F5-0ECE-42EB-8BF2-A4F708BDC2BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="887" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1046,8 +1046,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="P20" sqref="P20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>